<commit_message>
Trying inserting crack info
modifying data tables + clean script to have new crack features
</commit_message>
<xml_diff>
--- a/Cleaning_data/ManuallyCleanedData.xlsx
+++ b/Cleaning_data/ManuallyCleanedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samy/Desktop/S3/Data-Science-Project/Cleaning_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994259E1-4B3C-5F4F-8DD5-F80323AB2CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A48C6EE-69C5-AC49-A252-685890DC550A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CD9CC8B6-7F43-9E44-8EF2-1878F1CC02BE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{CD9CC8B6-7F43-9E44-8EF2-1878F1CC02BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5694,9 +5694,6 @@
     <t>parallel to hoizontal members_x001D_</t>
   </si>
   <si>
-    <t>parallel to all edges_x001D_paarellel to right member</t>
-  </si>
-  <si>
     <t>paarellel to right member_x001D_</t>
   </si>
   <si>
@@ -5715,9 +5712,6 @@
     <t>corner circle (quadrant) cracks (stress at corners)_x001D_parallel to all edges</t>
   </si>
   <si>
-    <t>parallel to left member_x001D_parallel to bottom member</t>
-  </si>
-  <si>
     <t>parallel to right member_x001D_</t>
   </si>
   <si>
@@ -5739,9 +5733,6 @@
     <t>parallel to cross bars_x001D_vertical cross bar</t>
   </si>
   <si>
-    <t>parallel to bottom member_x001D_parallel to cross bars</t>
-  </si>
-  <si>
     <t>parallel to left member_x001D_local</t>
   </si>
   <si>
@@ -6520,6 +6511,15 @@
   </si>
   <si>
     <t>at the support layer, dark shadows visible_x001D_at the right edge</t>
+  </si>
+  <si>
+    <t>parallel to all edges;paarellel to right member</t>
+  </si>
+  <si>
+    <t>parallel to left member;parallel to bottom member</t>
+  </si>
+  <si>
+    <t>parallel to bottom member;parallel to cross bars</t>
   </si>
 </sst>
 </file>
@@ -6923,8 +6923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41110769-F909-4249-923C-C513B87E37AD}">
   <dimension ref="A1:FE209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FC1" workbookViewId="0">
-      <selection activeCell="FD8" sqref="FD8"/>
+    <sheetView tabSelected="1" topLeftCell="FB1" workbookViewId="0">
+      <selection activeCell="FC1" sqref="FC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7444,13 +7444,13 @@
         <v>1855</v>
       </c>
       <c r="FC1" s="1" t="s">
-        <v>1884</v>
+        <v>1881</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>2035</v>
+        <v>2032</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>2112</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="2" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -7746,13 +7746,13 @@
         <v>157</v>
       </c>
       <c r="FC2" s="2" t="s">
-        <v>1885</v>
+        <v>1882</v>
       </c>
       <c r="FD2" s="2" t="s">
-        <v>2036</v>
+        <v>2033</v>
       </c>
       <c r="FE2" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="3" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -8030,13 +8030,13 @@
         <v>1856</v>
       </c>
       <c r="FC3" s="2" t="s">
-        <v>1886</v>
+        <v>1883</v>
       </c>
       <c r="FD3" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE3" s="2" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="4" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -8308,13 +8308,13 @@
         <v>157</v>
       </c>
       <c r="FC4" s="2" t="s">
-        <v>1887</v>
+        <v>1884</v>
       </c>
       <c r="FD4" s="2" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
       <c r="FE4" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="5" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -8622,13 +8622,13 @@
         <v>157</v>
       </c>
       <c r="FC5" s="2" t="s">
-        <v>1888</v>
+        <v>1885</v>
       </c>
       <c r="FD5" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE5" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="6" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -8891,10 +8891,10 @@
         <v>1857</v>
       </c>
       <c r="FC6" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD6" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE6" s="2" t="s">
         <v>391</v>
@@ -9165,13 +9165,13 @@
         <v>1858</v>
       </c>
       <c r="FC7" s="2" t="s">
-        <v>1890</v>
+        <v>1887</v>
       </c>
       <c r="FD7" s="2" t="s">
-        <v>2039</v>
+        <v>2036</v>
       </c>
       <c r="FE7" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="8" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -9450,13 +9450,13 @@
         <v>157</v>
       </c>
       <c r="FC8" s="2" t="s">
-        <v>1891</v>
+        <v>1888</v>
       </c>
       <c r="FD8" s="2" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="FE8" s="2" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="9" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -9737,13 +9737,13 @@
         <v>157</v>
       </c>
       <c r="FC9" s="2" t="s">
-        <v>1892</v>
+        <v>1889</v>
       </c>
       <c r="FD9" s="2" t="s">
-        <v>2041</v>
+        <v>2038</v>
       </c>
       <c r="FE9" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="10" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -10038,13 +10038,13 @@
         <v>1859</v>
       </c>
       <c r="FC10" s="2" t="s">
-        <v>1893</v>
+        <v>1890</v>
       </c>
       <c r="FD10" s="2" t="s">
-        <v>2042</v>
+        <v>2039</v>
       </c>
       <c r="FE10" s="2" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="11" spans="1:161" ht="51" x14ac:dyDescent="0.2">
@@ -10325,13 +10325,13 @@
         <v>1860</v>
       </c>
       <c r="FC11" s="2" t="s">
-        <v>1894</v>
+        <v>1891</v>
       </c>
       <c r="FD11" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE11" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="12" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -10464,13 +10464,13 @@
         <v>157</v>
       </c>
       <c r="FC12" s="2" t="s">
-        <v>2029</v>
+        <v>2026</v>
       </c>
       <c r="FD12" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE12" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="13" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -10760,13 +10760,13 @@
         <v>1860</v>
       </c>
       <c r="FC13" s="2" t="s">
-        <v>1895</v>
+        <v>1892</v>
       </c>
       <c r="FD13" s="2" t="s">
-        <v>2043</v>
+        <v>2040</v>
       </c>
       <c r="FE13" s="2" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="14" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -11026,13 +11026,13 @@
         <v>157</v>
       </c>
       <c r="FC14" s="2" t="s">
-        <v>1896</v>
+        <v>1893</v>
       </c>
       <c r="FD14" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE14" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="15" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -11312,13 +11312,13 @@
         <v>157</v>
       </c>
       <c r="FC15" s="2" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="FD15" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE15" s="2" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="16" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -11597,13 +11597,13 @@
         <v>157</v>
       </c>
       <c r="FC16" s="2" t="s">
-        <v>1898</v>
+        <v>1895</v>
       </c>
       <c r="FD16" s="2" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="FE16" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="17" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -11869,13 +11869,13 @@
         <v>1860</v>
       </c>
       <c r="FC17" s="2" t="s">
-        <v>1899</v>
+        <v>1896</v>
       </c>
       <c r="FD17" s="2" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
       <c r="FE17" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="18" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -12135,13 +12135,13 @@
         <v>1860</v>
       </c>
       <c r="FC18" s="2" t="s">
-        <v>1900</v>
+        <v>1897</v>
       </c>
       <c r="FD18" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE18" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="19" spans="1:161" x14ac:dyDescent="0.2">
@@ -12270,7 +12270,7 @@
         <v>157</v>
       </c>
       <c r="FC19" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD19" s="2" t="s">
         <v>1443</v>
@@ -12520,13 +12520,13 @@
         <v>1856</v>
       </c>
       <c r="FC20" s="2" t="s">
-        <v>1901</v>
+        <v>1898</v>
       </c>
       <c r="FD20" s="2" t="s">
-        <v>2046</v>
+        <v>2043</v>
       </c>
       <c r="FE20" s="2" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="21" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -12735,13 +12735,13 @@
         <v>157</v>
       </c>
       <c r="FC21" s="2" t="s">
-        <v>1902</v>
+        <v>1899</v>
       </c>
       <c r="FD21" s="2" t="s">
-        <v>2047</v>
+        <v>2044</v>
       </c>
       <c r="FE21" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="22" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -13008,10 +13008,10 @@
         <v>157</v>
       </c>
       <c r="FC22" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD22" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE22" s="2" t="s">
         <v>391</v>
@@ -13270,13 +13270,13 @@
         <v>157</v>
       </c>
       <c r="FC23" s="2" t="s">
-        <v>1903</v>
+        <v>1900</v>
       </c>
       <c r="FD23" s="2" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
       <c r="FE23" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="24" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -13426,13 +13426,13 @@
         <v>157</v>
       </c>
       <c r="FC24" s="2" t="s">
-        <v>2028</v>
+        <v>2025</v>
       </c>
       <c r="FD24" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE24" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="25" spans="1:161" x14ac:dyDescent="0.2">
@@ -13603,13 +13603,13 @@
         <v>157</v>
       </c>
       <c r="FC25" s="2" t="s">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="FD25" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE25" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="26" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -13879,13 +13879,13 @@
         <v>1861</v>
       </c>
       <c r="FC26" s="2" t="s">
-        <v>1905</v>
+        <v>1902</v>
       </c>
       <c r="FD26" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE26" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="27" spans="1:161" x14ac:dyDescent="0.2">
@@ -14057,13 +14057,13 @@
         <v>157</v>
       </c>
       <c r="FC27" s="2" t="s">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="FD27" s="2" t="s">
-        <v>2049</v>
+        <v>2046</v>
       </c>
       <c r="FE27" s="2" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="28" spans="1:161" x14ac:dyDescent="0.2">
@@ -14339,13 +14339,13 @@
         <v>1856</v>
       </c>
       <c r="FC28" s="2" t="s">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="FD28" s="2" t="s">
-        <v>2050</v>
+        <v>2047</v>
       </c>
       <c r="FE28" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="29" spans="1:161" x14ac:dyDescent="0.2">
@@ -14617,13 +14617,13 @@
         <v>157</v>
       </c>
       <c r="FC29" s="2" t="s">
-        <v>1908</v>
+        <v>1905</v>
       </c>
       <c r="FD29" s="2" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
       <c r="FE29" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="30" spans="1:161" x14ac:dyDescent="0.2">
@@ -14880,13 +14880,13 @@
         <v>1862</v>
       </c>
       <c r="FC30" s="2" t="s">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="FD30" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE30" s="2" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="31" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -15152,13 +15152,13 @@
         <v>1862</v>
       </c>
       <c r="FC31" s="2" t="s">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="FD31" s="2" t="s">
-        <v>2051</v>
+        <v>2048</v>
       </c>
       <c r="FE31" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="32" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -15322,10 +15322,10 @@
         <v>157</v>
       </c>
       <c r="FC32" s="2" t="s">
-        <v>1911</v>
+        <v>1908</v>
       </c>
       <c r="FD32" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE32" s="2" t="s">
         <v>391</v>
@@ -15561,13 +15561,13 @@
         <v>157</v>
       </c>
       <c r="FC33" s="2" t="s">
-        <v>1912</v>
+        <v>1909</v>
       </c>
       <c r="FD33" s="2" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
       <c r="FE33" s="2" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="34" spans="1:161" x14ac:dyDescent="0.2">
@@ -15794,13 +15794,13 @@
         <v>1856</v>
       </c>
       <c r="FC34" s="2" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
       <c r="FD34" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE34" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="35" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -15955,13 +15955,13 @@
         <v>157</v>
       </c>
       <c r="FC35" s="2" t="s">
-        <v>1914</v>
+        <v>1911</v>
       </c>
       <c r="FD35" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE35" s="2" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="36" spans="1:161" x14ac:dyDescent="0.2">
@@ -16221,13 +16221,13 @@
         <v>1863</v>
       </c>
       <c r="FC36" s="2" t="s">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="FD36" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE36" s="2" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="37" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -16477,13 +16477,13 @@
         <v>1863</v>
       </c>
       <c r="FC37" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD37" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE37" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="38" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -16737,13 +16737,13 @@
         <v>1864</v>
       </c>
       <c r="FC38" s="2" t="s">
-        <v>1916</v>
+        <v>1913</v>
       </c>
       <c r="FD38" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE38" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="39" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -16985,10 +16985,10 @@
         <v>1862</v>
       </c>
       <c r="FC39" s="2" t="s">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="FD39" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE39" s="2" t="s">
         <v>391</v>
@@ -17256,13 +17256,13 @@
         <v>1856</v>
       </c>
       <c r="FC40" s="2" t="s">
-        <v>1918</v>
+        <v>1915</v>
       </c>
       <c r="FD40" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE40" s="2" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="41" spans="1:161" x14ac:dyDescent="0.2">
@@ -17515,13 +17515,13 @@
         <v>1860</v>
       </c>
       <c r="FC41" s="2" t="s">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="FD41" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE41" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="42" spans="1:161" x14ac:dyDescent="0.2">
@@ -17777,16 +17777,16 @@
         <v>1819</v>
       </c>
       <c r="FB42" s="2" t="s">
-        <v>1865</v>
+        <v>2138</v>
       </c>
       <c r="FC42" s="2" t="s">
-        <v>1920</v>
+        <v>1917</v>
       </c>
       <c r="FD42" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE42" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="43" spans="1:161" x14ac:dyDescent="0.2">
@@ -18038,10 +18038,10 @@
         <v>157</v>
       </c>
       <c r="FC43" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD43" s="2" t="s">
-        <v>2052</v>
+        <v>2049</v>
       </c>
       <c r="FE43" s="2" t="s">
         <v>391</v>
@@ -18217,13 +18217,13 @@
         <v>1860</v>
       </c>
       <c r="FC44" s="2" t="s">
-        <v>1921</v>
+        <v>1918</v>
       </c>
       <c r="FD44" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE44" s="2" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="45" spans="1:161" x14ac:dyDescent="0.2">
@@ -18478,16 +18478,16 @@
         <v>1817</v>
       </c>
       <c r="FB45" s="2" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="FC45" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD45" s="2" t="s">
-        <v>2053</v>
+        <v>2050</v>
       </c>
       <c r="FE45" s="2" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="46" spans="1:161" x14ac:dyDescent="0.2">
@@ -18622,10 +18622,10 @@
         <v>1860</v>
       </c>
       <c r="FC46" s="2" t="s">
-        <v>1922</v>
+        <v>1919</v>
       </c>
       <c r="FD46" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE46" s="2" t="s">
         <v>391</v>
@@ -18762,10 +18762,10 @@
         <v>157</v>
       </c>
       <c r="FC47" s="2" t="s">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="FD47" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE47" s="2" t="s">
         <v>391</v>
@@ -19005,13 +19005,13 @@
         <v>1856</v>
       </c>
       <c r="FC48" s="2" t="s">
-        <v>1923</v>
+        <v>1920</v>
       </c>
       <c r="FD48" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE48" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="49" spans="1:161" x14ac:dyDescent="0.2">
@@ -19243,16 +19243,16 @@
         <v>129</v>
       </c>
       <c r="FB49" s="2" t="s">
-        <v>1883</v>
+        <v>1880</v>
       </c>
       <c r="FC49" s="2" t="s">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="FD49" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE49" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="50" spans="1:161" x14ac:dyDescent="0.2">
@@ -19425,13 +19425,13 @@
         <v>157</v>
       </c>
       <c r="FC50" s="2" t="s">
-        <v>1924</v>
+        <v>1921</v>
       </c>
       <c r="FD50" s="2" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="FE50" s="2" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="51" spans="1:161" x14ac:dyDescent="0.2">
@@ -19609,16 +19609,16 @@
         <v>1822</v>
       </c>
       <c r="FB51" s="2" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="FC51" s="2" t="s">
-        <v>1925</v>
+        <v>1922</v>
       </c>
       <c r="FD51" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE51" s="2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="52" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -19881,13 +19881,13 @@
         <v>157</v>
       </c>
       <c r="FC52" s="2" t="s">
-        <v>1926</v>
+        <v>1923</v>
       </c>
       <c r="FD52" s="2" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="FE52" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="53" spans="1:161" x14ac:dyDescent="0.2">
@@ -20076,16 +20076,16 @@
         <v>1550</v>
       </c>
       <c r="FB53" s="2" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="FC53" s="2" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
       <c r="FD53" s="2" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
       <c r="FE53" s="2" t="s">
-        <v>2130</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="54" spans="1:161" x14ac:dyDescent="0.2">
@@ -20261,13 +20261,13 @@
         <v>157</v>
       </c>
       <c r="FC54" s="2" t="s">
-        <v>1928</v>
+        <v>1925</v>
       </c>
       <c r="FD54" s="2" t="s">
-        <v>2055</v>
+        <v>2052</v>
       </c>
       <c r="FE54" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="55" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -20543,13 +20543,13 @@
         <v>1864</v>
       </c>
       <c r="FC55" s="2" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="FD55" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE55" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="56" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -20821,13 +20821,13 @@
         <v>157</v>
       </c>
       <c r="FC56" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD56" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE56" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="57" spans="1:161" x14ac:dyDescent="0.2">
@@ -21004,13 +21004,13 @@
         <v>1862</v>
       </c>
       <c r="FC57" s="2" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
       <c r="FD57" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE57" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="58" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -21268,13 +21268,13 @@
         <v>1862</v>
       </c>
       <c r="FC58" s="2" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
       <c r="FD58" s="2" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
       <c r="FE58" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="59" spans="1:161" x14ac:dyDescent="0.2">
@@ -21460,13 +21460,13 @@
         <v>157</v>
       </c>
       <c r="FC59" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD59" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE59" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="60" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -21630,13 +21630,13 @@
         <v>157</v>
       </c>
       <c r="FC60" s="2" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
       <c r="FD60" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE60" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="61" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -21808,13 +21808,13 @@
         <v>157</v>
       </c>
       <c r="FC61" s="2" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
       <c r="FD61" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE61" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="62" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -21986,13 +21986,13 @@
         <v>157</v>
       </c>
       <c r="FC62" s="2" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
       <c r="FD62" s="2" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="FE62" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="63" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -22168,10 +22168,10 @@
         <v>157</v>
       </c>
       <c r="FC63" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD63" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE63" s="2" t="s">
         <v>391</v>
@@ -22354,10 +22354,10 @@
         <v>157</v>
       </c>
       <c r="FC64" s="2" t="s">
-        <v>1934</v>
+        <v>1931</v>
       </c>
       <c r="FD64" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE64" s="2" t="s">
         <v>391</v>
@@ -22600,10 +22600,10 @@
         <v>157</v>
       </c>
       <c r="FC65" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD65" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE65" s="2" t="s">
         <v>391</v>
@@ -22763,13 +22763,13 @@
         <v>157</v>
       </c>
       <c r="FC66" s="2" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="FD66" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE66" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="67" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -22938,13 +22938,13 @@
         <v>157</v>
       </c>
       <c r="FC67" s="2" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
       <c r="FD67" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE67" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="68" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -23099,10 +23099,10 @@
         <v>157</v>
       </c>
       <c r="FC68" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD68" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE68" s="2" t="s">
         <v>391</v>
@@ -23374,13 +23374,13 @@
         <v>1860</v>
       </c>
       <c r="FC69" s="2" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="FD69" s="2" t="s">
-        <v>2056</v>
+        <v>2053</v>
       </c>
       <c r="FE69" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="70" spans="1:161" x14ac:dyDescent="0.2">
@@ -23544,13 +23544,13 @@
         <v>157</v>
       </c>
       <c r="FC70" s="2" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
       <c r="FD70" s="2" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
       <c r="FE70" s="2" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="71" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -23717,10 +23717,10 @@
         <v>157</v>
       </c>
       <c r="FC71" s="2" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
       <c r="FD71" s="2" t="s">
-        <v>2056</v>
+        <v>2053</v>
       </c>
       <c r="FE71" s="2" t="s">
         <v>391</v>
@@ -23884,13 +23884,13 @@
         <v>1860</v>
       </c>
       <c r="FC72" s="2" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="FD72" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE72" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="73" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -24075,13 +24075,13 @@
         <v>157</v>
       </c>
       <c r="FC73" s="2" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
       <c r="FD73" s="2" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
       <c r="FE73" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="74" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -24339,10 +24339,10 @@
         <v>157</v>
       </c>
       <c r="FC74" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD74" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE74" s="2" t="s">
         <v>391</v>
@@ -24507,13 +24507,13 @@
         <v>157</v>
       </c>
       <c r="FC75" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD75" s="2" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
       <c r="FE75" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="76" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -24804,10 +24804,10 @@
         <v>1856</v>
       </c>
       <c r="FC76" s="2" t="s">
-        <v>1941</v>
+        <v>1938</v>
       </c>
       <c r="FD76" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE76" s="2" t="s">
         <v>391</v>
@@ -24990,10 +24990,10 @@
         <v>157</v>
       </c>
       <c r="FC77" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD77" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE77" s="2" t="s">
         <v>391</v>
@@ -25192,13 +25192,13 @@
         <v>157</v>
       </c>
       <c r="FC78" s="2" t="s">
-        <v>1942</v>
+        <v>1939</v>
       </c>
       <c r="FD78" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE78" s="2" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="79" spans="1:161" x14ac:dyDescent="0.2">
@@ -25450,16 +25450,16 @@
         <v>1809</v>
       </c>
       <c r="FB79" s="2" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="FC79" s="2" t="s">
-        <v>1943</v>
+        <v>1940</v>
       </c>
       <c r="FD79" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE79" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="80" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -25743,13 +25743,13 @@
         <v>1860</v>
       </c>
       <c r="FC80" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD80" s="2" t="s">
-        <v>2059</v>
+        <v>2056</v>
       </c>
       <c r="FE80" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="81" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -25912,13 +25912,13 @@
         <v>157</v>
       </c>
       <c r="FC81" s="2" t="s">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="FD81" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE81" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="82" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -26152,13 +26152,13 @@
         <v>1856</v>
       </c>
       <c r="FC82" s="2" t="s">
-        <v>1944</v>
+        <v>1941</v>
       </c>
       <c r="FD82" s="2" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
       <c r="FE82" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="83" spans="1:161" x14ac:dyDescent="0.2">
@@ -26370,13 +26370,13 @@
         <v>157</v>
       </c>
       <c r="FC83" s="2" t="s">
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="FD83" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE83" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="84" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -26616,16 +26616,16 @@
         <v>1807</v>
       </c>
       <c r="FB84" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="FC84" s="2" t="s">
-        <v>1945</v>
+        <v>1942</v>
       </c>
       <c r="FD84" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE84" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="85" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -26865,16 +26865,16 @@
         <v>1807</v>
       </c>
       <c r="FB85" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="FC85" s="2" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
       <c r="FD85" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE85" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="86" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -27139,10 +27139,10 @@
         <v>157</v>
       </c>
       <c r="FC86" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD86" s="2" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="FE86" s="2" t="s">
         <v>391</v>
@@ -27306,13 +27306,13 @@
         <v>157</v>
       </c>
       <c r="FC87" s="2" t="s">
-        <v>1928</v>
+        <v>1925</v>
       </c>
       <c r="FD87" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE87" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="88" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -27494,10 +27494,10 @@
         <v>157</v>
       </c>
       <c r="FC88" s="2" t="s">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="FD88" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE88" s="2" t="s">
         <v>391</v>
@@ -27679,13 +27679,13 @@
         <v>157</v>
       </c>
       <c r="FC89" s="2" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
       <c r="FD89" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE89" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="90" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -27872,13 +27872,13 @@
         <v>157</v>
       </c>
       <c r="FC90" s="2" t="s">
-        <v>1948</v>
+        <v>1945</v>
       </c>
       <c r="FD90" s="2" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
       <c r="FE90" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="91" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -28114,13 +28114,13 @@
         <v>157</v>
       </c>
       <c r="FC91" s="2" t="s">
-        <v>1949</v>
+        <v>1946</v>
       </c>
       <c r="FD91" s="2" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
       <c r="FE91" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="92" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -28397,16 +28397,16 @@
         <v>1815</v>
       </c>
       <c r="FB92" s="2" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="FC92" s="2" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
       <c r="FD92" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE92" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="93" spans="1:161" x14ac:dyDescent="0.2">
@@ -28589,10 +28589,10 @@
         <v>157</v>
       </c>
       <c r="FC93" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD93" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE93" s="2" t="s">
         <v>391</v>
@@ -28867,13 +28867,13 @@
         <v>1860</v>
       </c>
       <c r="FC94" s="2" t="s">
-        <v>1951</v>
+        <v>1948</v>
       </c>
       <c r="FD94" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE94" s="2" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="95" spans="1:161" x14ac:dyDescent="0.2">
@@ -29053,16 +29053,16 @@
         <v>1809</v>
       </c>
       <c r="FB95" s="2" t="s">
-        <v>1872</v>
+        <v>2139</v>
       </c>
       <c r="FC95" s="2" t="s">
-        <v>1952</v>
+        <v>1949</v>
       </c>
       <c r="FD95" s="2" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
       <c r="FE95" s="2" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="96" spans="1:161" x14ac:dyDescent="0.2">
@@ -29234,13 +29234,13 @@
         <v>157</v>
       </c>
       <c r="FC96" s="2" t="s">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="FD96" s="2" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
       <c r="FE96" s="2" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="97" spans="1:161" x14ac:dyDescent="0.2">
@@ -29473,13 +29473,13 @@
         <v>157</v>
       </c>
       <c r="FC97" s="2" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
       <c r="FD97" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE97" s="2" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="98" spans="1:161" x14ac:dyDescent="0.2">
@@ -29700,10 +29700,10 @@
         <v>157</v>
       </c>
       <c r="FC98" s="2" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="FD98" s="2" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
       <c r="FE98" s="2" t="s">
         <v>391</v>
@@ -29974,13 +29974,13 @@
         <v>1860</v>
       </c>
       <c r="FC99" s="2" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="FD99" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE99" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="100" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -30200,13 +30200,13 @@
         <v>1860</v>
       </c>
       <c r="FC100" s="2" t="s">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="FD100" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE100" s="2" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="101" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -30476,13 +30476,13 @@
         <v>157</v>
       </c>
       <c r="FC101" s="2" t="s">
-        <v>1958</v>
+        <v>1955</v>
       </c>
       <c r="FD101" s="2" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
       <c r="FE101" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="102" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -30728,16 +30728,16 @@
         <v>1809</v>
       </c>
       <c r="FB102" s="2" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="FC102" s="2" t="s">
-        <v>1949</v>
+        <v>1946</v>
       </c>
       <c r="FD102" s="2" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="FE102" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="103" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -30978,13 +30978,13 @@
         <v>1860</v>
       </c>
       <c r="FC103" s="2" t="s">
-        <v>1959</v>
+        <v>1956</v>
       </c>
       <c r="FD103" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE103" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="104" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -31214,10 +31214,10 @@
         <v>157</v>
       </c>
       <c r="FC104" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD104" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE104" s="2" t="s">
         <v>391</v>
@@ -31480,13 +31480,13 @@
         <v>157</v>
       </c>
       <c r="FC105" s="2" t="s">
-        <v>1960</v>
+        <v>1957</v>
       </c>
       <c r="FD105" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE105" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="106" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -31721,13 +31721,13 @@
         <v>1860</v>
       </c>
       <c r="FC106" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD106" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE106" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="107" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -31996,13 +31996,13 @@
         <v>1857</v>
       </c>
       <c r="FC107" s="2" t="s">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="FD107" s="2" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
       <c r="FE107" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="108" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -32257,13 +32257,13 @@
         <v>157</v>
       </c>
       <c r="FC108" s="2" t="s">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="FD108" s="2" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
       <c r="FE108" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="109" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -32551,13 +32551,13 @@
         <v>1860</v>
       </c>
       <c r="FC109" s="2" t="s">
-        <v>1963</v>
+        <v>1960</v>
       </c>
       <c r="FD109" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE109" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="110" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -32851,13 +32851,13 @@
         <v>157</v>
       </c>
       <c r="FC110" s="2" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="FD110" s="2" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
       <c r="FE110" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="111" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -33093,13 +33093,13 @@
         <v>1862</v>
       </c>
       <c r="FC111" s="2" t="s">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="FD111" s="2" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
       <c r="FE111" s="2" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="112" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -33328,10 +33328,10 @@
         <v>157</v>
       </c>
       <c r="FC112" s="2" t="s">
-        <v>1966</v>
+        <v>1963</v>
       </c>
       <c r="FD112" s="2" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
       <c r="FE112" s="2" t="s">
         <v>391</v>
@@ -33580,13 +33580,13 @@
         <v>157</v>
       </c>
       <c r="FC113" s="2" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="FD113" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE113" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="114" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -33760,13 +33760,13 @@
         <v>157</v>
       </c>
       <c r="FC114" s="2" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="FD114" s="2" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="FE114" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="115" spans="1:161" x14ac:dyDescent="0.2">
@@ -33952,13 +33952,13 @@
         <v>157</v>
       </c>
       <c r="FC115" s="2" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
       <c r="FD115" s="2" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
       <c r="FE115" s="2" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="116" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -34183,13 +34183,13 @@
         <v>1860</v>
       </c>
       <c r="FC116" s="2" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="FD116" s="2" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="FE116" s="2" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="117" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -34446,13 +34446,13 @@
         <v>1857</v>
       </c>
       <c r="FC117" s="2" t="s">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="FD117" s="2" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="FE117" s="2" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="118" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -34693,16 +34693,16 @@
         <v>1817</v>
       </c>
       <c r="FB118" s="2" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="FC118" s="2" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
       <c r="FD118" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE118" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="119" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -34942,16 +34942,16 @@
         <v>129</v>
       </c>
       <c r="FB119" s="2" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="FC119" s="2" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="FD119" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE119" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="120" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -35127,13 +35127,13 @@
         <v>157</v>
       </c>
       <c r="FC120" s="2" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="FD120" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE120" s="2" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="121" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -35311,10 +35311,10 @@
         <v>157</v>
       </c>
       <c r="FC121" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD121" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE121" s="2" t="s">
         <v>391</v>
@@ -35487,10 +35487,10 @@
         <v>157</v>
       </c>
       <c r="FC122" s="2" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="FD122" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE122" s="2" t="s">
         <v>391</v>
@@ -35748,13 +35748,13 @@
         <v>1862</v>
       </c>
       <c r="FC123" s="2" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="FD123" s="2" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
       <c r="FE123" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="124" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -35933,13 +35933,13 @@
         <v>157</v>
       </c>
       <c r="FC124" s="2" t="s">
-        <v>1977</v>
+        <v>1974</v>
       </c>
       <c r="FD124" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE124" s="2" t="s">
-        <v>2138</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="125" spans="1:161" x14ac:dyDescent="0.2">
@@ -36050,10 +36050,10 @@
         <v>157</v>
       </c>
       <c r="FC125" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD125" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE125" s="2" t="s">
         <v>391</v>
@@ -36174,10 +36174,10 @@
         <v>157</v>
       </c>
       <c r="FC126" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD126" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE126" s="2" t="s">
         <v>391</v>
@@ -36354,10 +36354,10 @@
         <v>157</v>
       </c>
       <c r="FC127" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD127" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE127" s="2" t="s">
         <v>391</v>
@@ -36620,13 +36620,13 @@
         <v>157</v>
       </c>
       <c r="FC128" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD128" s="2" t="s">
-        <v>2076</v>
+        <v>2073</v>
       </c>
       <c r="FE128" s="2" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="129" spans="1:161" x14ac:dyDescent="0.2">
@@ -36772,10 +36772,10 @@
         <v>157</v>
       </c>
       <c r="FC129" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD129" s="2" t="s">
-        <v>2077</v>
+        <v>2074</v>
       </c>
       <c r="FE129" s="2" t="s">
         <v>391</v>
@@ -36932,13 +36932,13 @@
         <v>157</v>
       </c>
       <c r="FC130" s="2" t="s">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="FD130" s="2" t="s">
-        <v>2078</v>
+        <v>2075</v>
       </c>
       <c r="FE130" s="2" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="131" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -37205,13 +37205,13 @@
         <v>157</v>
       </c>
       <c r="FC131" s="2" t="s">
-        <v>1980</v>
+        <v>1977</v>
       </c>
       <c r="FD131" s="2" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
       <c r="FE131" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="132" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -37482,10 +37482,10 @@
         <v>157</v>
       </c>
       <c r="FC132" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD132" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE132" s="2" t="s">
         <v>391</v>
@@ -37678,13 +37678,13 @@
         <v>157</v>
       </c>
       <c r="FC133" s="2" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="FD133" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE133" s="2" t="s">
-        <v>2139</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="134" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -37876,13 +37876,13 @@
         <v>157</v>
       </c>
       <c r="FC134" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD134" s="2" t="s">
-        <v>2079</v>
+        <v>2076</v>
       </c>
       <c r="FE134" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="135" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -38042,13 +38042,13 @@
         <v>157</v>
       </c>
       <c r="FC135" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD135" s="2" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="FE135" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="136" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -38198,13 +38198,13 @@
         <v>157</v>
       </c>
       <c r="FC136" s="2" t="s">
-        <v>1982</v>
+        <v>1979</v>
       </c>
       <c r="FD136" s="2" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="FE136" s="2" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="137" spans="1:161" x14ac:dyDescent="0.2">
@@ -38389,16 +38389,16 @@
         <v>1808</v>
       </c>
       <c r="FB137" s="2" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="FC137" s="2" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="FD137" s="2" t="s">
         <v>1443</v>
       </c>
       <c r="FE137" s="2" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="138" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -38549,13 +38549,13 @@
         <v>157</v>
       </c>
       <c r="FC138" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD138" s="2" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="FE138" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="139" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -38712,13 +38712,13 @@
         <v>157</v>
       </c>
       <c r="FC139" s="2" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="FD139" s="2" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="FE139" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="140" spans="1:161" x14ac:dyDescent="0.2">
@@ -38891,13 +38891,13 @@
         <v>157</v>
       </c>
       <c r="FC140" s="2" t="s">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="FD140" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE140" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="141" spans="1:161" x14ac:dyDescent="0.2">
@@ -39070,13 +39070,13 @@
         <v>1864</v>
       </c>
       <c r="FC141" s="2" t="s">
-        <v>1986</v>
+        <v>1983</v>
       </c>
       <c r="FD141" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE141" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="142" spans="1:161" x14ac:dyDescent="0.2">
@@ -39207,13 +39207,13 @@
         <v>157</v>
       </c>
       <c r="FC142" s="2" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="FD142" s="2" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="FE142" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="143" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -39398,13 +39398,13 @@
         <v>157</v>
       </c>
       <c r="FC143" s="2" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="FD143" s="2" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
       <c r="FE143" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="144" spans="1:161" x14ac:dyDescent="0.2">
@@ -39547,10 +39547,10 @@
         <v>157</v>
       </c>
       <c r="FC144" s="2" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="FD144" s="2" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
       <c r="FE144" s="2" t="s">
         <v>157</v>
@@ -39805,16 +39805,16 @@
         <v>1820</v>
       </c>
       <c r="FB145" s="2" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="FC145" s="2" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="FD145" s="2" t="s">
-        <v>2056</v>
+        <v>2053</v>
       </c>
       <c r="FE145" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="146" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -40086,13 +40086,13 @@
         <v>1860</v>
       </c>
       <c r="FC146" s="2" t="s">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="FD146" s="2" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="FE146" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="147" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -40355,13 +40355,13 @@
         <v>157</v>
       </c>
       <c r="FC147" s="2" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="FD147" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE147" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="148" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -40608,13 +40608,13 @@
         <v>1856</v>
       </c>
       <c r="FC148" s="2" t="s">
-        <v>1992</v>
+        <v>1989</v>
       </c>
       <c r="FD148" s="2" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="FE148" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="149" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -40751,13 +40751,13 @@
         <v>157</v>
       </c>
       <c r="FC149" s="2" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="FD149" s="2" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="FE149" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="150" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -41024,13 +41024,13 @@
         <v>157</v>
       </c>
       <c r="FC150" s="2" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="FD150" s="2" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="FE150" s="2" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="151" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -41301,10 +41301,10 @@
         <v>157</v>
       </c>
       <c r="FC151" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD151" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE151" s="2" t="s">
         <v>391</v>
@@ -41574,10 +41574,10 @@
         <v>157</v>
       </c>
       <c r="FC152" s="2" t="s">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="FD152" s="2" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="FE152" s="2" t="s">
         <v>157</v>
@@ -41830,13 +41830,13 @@
         <v>157</v>
       </c>
       <c r="FC153" s="2" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="FD153" s="2" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="FE153" s="2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="154" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -42075,16 +42075,16 @@
         <v>1807</v>
       </c>
       <c r="FB154" s="2" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="FC154" s="2" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="FD154" s="2" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="FE154" s="2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="155" spans="1:161" x14ac:dyDescent="0.2">
@@ -42266,13 +42266,13 @@
         <v>1862</v>
       </c>
       <c r="FC155" s="2" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="FD155" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE155" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="156" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -42525,13 +42525,13 @@
         <v>157</v>
       </c>
       <c r="FC156" s="2" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="FD156" s="2" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
       <c r="FE156" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="157" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -42698,13 +42698,13 @@
         <v>1857</v>
       </c>
       <c r="FC157" s="2" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="FD157" s="2" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="FE157" s="2" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="158" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -42960,13 +42960,13 @@
         <v>1856</v>
       </c>
       <c r="FC158" s="2" t="s">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="FD158" s="2" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="FE158" s="2" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="159" spans="1:161" x14ac:dyDescent="0.2">
@@ -43122,13 +43122,13 @@
         <v>157</v>
       </c>
       <c r="FC159" s="2" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="FD159" s="2" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
       <c r="FE159" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="160" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -43379,16 +43379,16 @@
         <v>1807</v>
       </c>
       <c r="FB160" s="2" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="FC160" s="2" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="FD160" s="2" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="FE160" s="2" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="161" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -43528,13 +43528,13 @@
         <v>157</v>
       </c>
       <c r="FC161" s="2" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="FD161" s="2" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="FE161" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="162" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -43786,16 +43786,16 @@
         <v>1815</v>
       </c>
       <c r="FB162" s="2" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="FC162" s="2" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="FD162" s="2" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="FE162" s="2" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="163" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -43939,13 +43939,13 @@
         <v>157</v>
       </c>
       <c r="FC163" s="2" t="s">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="FD163" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE163" s="2" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="164" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -44194,13 +44194,13 @@
         <v>157</v>
       </c>
       <c r="FC164" s="2" t="s">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="FD164" s="2" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
       <c r="FE164" s="2" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="165" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -44427,13 +44427,13 @@
         <v>157</v>
       </c>
       <c r="FC165" s="2" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="FD165" s="2" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="FE165" s="2" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="166" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -44587,13 +44587,13 @@
         <v>157</v>
       </c>
       <c r="FC166" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD166" s="2" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
       <c r="FE166" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="167" spans="1:161" x14ac:dyDescent="0.2">
@@ -44750,16 +44750,16 @@
         <v>1807</v>
       </c>
       <c r="FB167" s="2" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="FC167" s="2" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="FD167" s="2" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
       <c r="FE167" s="2" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="168" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -44991,10 +44991,10 @@
         <v>157</v>
       </c>
       <c r="FC168" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD168" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE168" s="2" t="s">
         <v>391</v>
@@ -45250,13 +45250,13 @@
         <v>157</v>
       </c>
       <c r="FC169" s="2" t="s">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="FD169" s="2" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
       <c r="FE169" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="170" spans="1:161" x14ac:dyDescent="0.2">
@@ -45505,13 +45505,13 @@
         <v>157</v>
       </c>
       <c r="FC170" s="2" t="s">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="FD170" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE170" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="171" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -45648,13 +45648,13 @@
         <v>157</v>
       </c>
       <c r="FC171" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD171" s="2" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="FE171" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="172" spans="1:161" x14ac:dyDescent="0.2">
@@ -45789,16 +45789,16 @@
         <v>1809</v>
       </c>
       <c r="FB172" s="2" t="s">
-        <v>1880</v>
+        <v>2140</v>
       </c>
       <c r="FC172" s="2" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="FD172" s="2" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="FE172" s="2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="173" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -45946,13 +45946,13 @@
         <v>157</v>
       </c>
       <c r="FC173" s="2" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="FD173" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE173" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="174" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -46107,13 +46107,13 @@
         <v>157</v>
       </c>
       <c r="FC174" s="2" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="FD174" s="2" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="FE174" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="175" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -46352,7 +46352,7 @@
         <v>157</v>
       </c>
       <c r="FC175" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD175" s="2" t="s">
         <v>1443</v>
@@ -46597,13 +46597,13 @@
         <v>157</v>
       </c>
       <c r="FC176" s="2" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="FD176" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE176" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="177" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -46751,13 +46751,13 @@
         <v>157</v>
       </c>
       <c r="FC177" s="2" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="FD177" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE177" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="178" spans="1:161" x14ac:dyDescent="0.2">
@@ -46912,13 +46912,13 @@
         <v>157</v>
       </c>
       <c r="FC178" s="2" t="s">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="FD178" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE178" s="2" t="s">
-        <v>2140</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="179" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -47076,13 +47076,13 @@
         <v>157</v>
       </c>
       <c r="FC179" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD179" s="2" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="FE179" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="180" spans="1:161" x14ac:dyDescent="0.2">
@@ -47229,13 +47229,13 @@
         <v>157</v>
       </c>
       <c r="FC180" s="2" t="s">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="FD180" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE180" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="181" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -47382,13 +47382,13 @@
         <v>157</v>
       </c>
       <c r="FC181" s="2" t="s">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="FD181" s="2" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
       <c r="FE181" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="182" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -47531,13 +47531,13 @@
         <v>157</v>
       </c>
       <c r="FC182" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD182" s="2" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="FE182" s="2" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="183" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -47684,10 +47684,10 @@
         <v>157</v>
       </c>
       <c r="FC183" s="2" t="s">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="FD183" s="2" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="FE183" s="2" t="s">
         <v>157</v>
@@ -47848,13 +47848,13 @@
         <v>157</v>
       </c>
       <c r="FC184" s="2" t="s">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="FD184" s="2" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
       <c r="FE184" s="2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="185" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -47996,10 +47996,10 @@
         <v>157</v>
       </c>
       <c r="FC185" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD185" s="2" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
       <c r="FE185" s="2" t="s">
         <v>391</v>
@@ -48139,10 +48139,10 @@
         <v>157</v>
       </c>
       <c r="FC186" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD186" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE186" s="2" t="s">
         <v>391</v>
@@ -48286,10 +48286,10 @@
         <v>157</v>
       </c>
       <c r="FC187" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD187" s="2" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
       <c r="FE187" s="2" t="s">
         <v>391</v>
@@ -48457,13 +48457,13 @@
         <v>157</v>
       </c>
       <c r="FC188" s="2" t="s">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="FD188" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE188" s="2" t="s">
-        <v>2138</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="189" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -48718,13 +48718,13 @@
         <v>157</v>
       </c>
       <c r="FC189" s="2" t="s">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="FD189" s="2" t="s">
-        <v>2105</v>
+        <v>2102</v>
       </c>
       <c r="FE189" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="190" spans="1:161" x14ac:dyDescent="0.2">
@@ -48902,10 +48902,10 @@
         <v>1860</v>
       </c>
       <c r="FC190" s="2" t="s">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="FD190" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE190" s="2" t="s">
         <v>157</v>
@@ -49057,13 +49057,13 @@
         <v>157</v>
       </c>
       <c r="FC191" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD191" s="2" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="FE191" s="2" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="192" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -49302,13 +49302,13 @@
         <v>157</v>
       </c>
       <c r="FC192" s="2" t="s">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="FD192" s="2" t="s">
-        <v>2106</v>
+        <v>2103</v>
       </c>
       <c r="FE192" s="2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="193" spans="1:161" x14ac:dyDescent="0.2">
@@ -49471,13 +49471,13 @@
         <v>157</v>
       </c>
       <c r="FC193" s="2" t="s">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="FD193" s="2" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="FE193" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="194" spans="1:161" x14ac:dyDescent="0.2">
@@ -49717,13 +49717,13 @@
         <v>157</v>
       </c>
       <c r="FC194" s="2" t="s">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="FD194" s="2" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="FE194" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="195" spans="1:161" x14ac:dyDescent="0.2">
@@ -49871,13 +49871,13 @@
         <v>157</v>
       </c>
       <c r="FC195" s="2" t="s">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="FD195" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE195" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="196" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -50026,13 +50026,13 @@
         <v>157</v>
       </c>
       <c r="FC196" s="2" t="s">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="FD196" s="2" t="s">
-        <v>2107</v>
+        <v>2104</v>
       </c>
       <c r="FE196" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="197" spans="1:161" x14ac:dyDescent="0.2">
@@ -50274,16 +50274,16 @@
         <v>129</v>
       </c>
       <c r="FB197" s="2" t="s">
-        <v>1881</v>
+        <v>1878</v>
       </c>
       <c r="FC197" s="2" t="s">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="FD197" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE197" s="2" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="198" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -50539,16 +50539,16 @@
         <v>1809</v>
       </c>
       <c r="FB198" s="2" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="FC198" s="2" t="s">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="FD198" s="2" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
       <c r="FE198" s="2" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="199" spans="1:161" x14ac:dyDescent="0.2">
@@ -50701,10 +50701,10 @@
         <v>157</v>
       </c>
       <c r="FC199" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD199" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE199" s="2" t="s">
         <v>157</v>
@@ -50863,10 +50863,10 @@
         <v>157</v>
       </c>
       <c r="FC200" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD200" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE200" s="2" t="s">
         <v>391</v>
@@ -51102,16 +51102,16 @@
         <v>97</v>
       </c>
       <c r="FB201" s="2" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="FC201" s="2" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="FD201" s="2" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="FE201" s="2" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="202" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -51263,13 +51263,13 @@
         <v>157</v>
       </c>
       <c r="FC202" s="2" t="s">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="FD202" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE202" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="203" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -51417,13 +51417,13 @@
         <v>157</v>
       </c>
       <c r="FC203" s="2" t="s">
-        <v>2030</v>
+        <v>2027</v>
       </c>
       <c r="FD203" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE203" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="204" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -51675,10 +51675,10 @@
         <v>157</v>
       </c>
       <c r="FC204" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD204" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE204" s="2" t="s">
         <v>391</v>
@@ -51934,16 +51934,16 @@
         <v>1809</v>
       </c>
       <c r="FB205" s="2" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
       <c r="FC205" s="2" t="s">
-        <v>2031</v>
+        <v>2028</v>
       </c>
       <c r="FD205" s="2" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="FE205" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="206" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -52185,13 +52185,13 @@
         <v>1860</v>
       </c>
       <c r="FC206" s="2" t="s">
-        <v>2032</v>
+        <v>2029</v>
       </c>
       <c r="FD206" s="2" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
       <c r="FE206" s="2" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="207" spans="1:161" ht="17" x14ac:dyDescent="0.2">
@@ -52435,13 +52435,13 @@
         <v>157</v>
       </c>
       <c r="FC207" s="2" t="s">
-        <v>2033</v>
+        <v>2030</v>
       </c>
       <c r="FD207" s="2" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="FE207" s="2" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="208" spans="1:161" x14ac:dyDescent="0.2">
@@ -52687,10 +52687,10 @@
         <v>1862</v>
       </c>
       <c r="FC208" s="2" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="FD208" s="2" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
       <c r="FE208" s="2" t="s">
         <v>157</v>
@@ -52946,13 +52946,13 @@
         <v>1860</v>
       </c>
       <c r="FC209" s="2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="FD209" s="2" t="s">
         <v>2034</v>
       </c>
-      <c r="FD209" s="2" t="s">
-        <v>2037</v>
-      </c>
       <c r="FE209" s="2" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>